<commit_message>
Adding to the best practises file
</commit_message>
<xml_diff>
--- a/Best Practises/General guidelines for every project.xlsx
+++ b/Best Practises/General guidelines for every project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankush.bhardwaj\Desktop\Personal\Miscellaneous\Best Practises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87CA520-0DCA-4FA7-9CEC-38D3BC3320E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A889B6-C183-4EBB-A594-6EE80FEB8E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Main Point </t>
   </si>
@@ -36,9 +36,6 @@
     <t>Make a text/excel file for all the important links</t>
   </si>
   <si>
-    <t xml:space="preserve">Make a excel to mention run time, input data size and other important attributes </t>
-  </si>
-  <si>
     <t>Make the main working directory based on the TAMLEP folder structure</t>
   </si>
   <si>
@@ -67,6 +64,25 @@
   </si>
   <si>
     <t>Write code in both pyspark and pandas</t>
+  </si>
+  <si>
+    <t>Write output of each function at some place to avoid testing remaining functions from start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make a excel to mention experiments run time, 
+input data size and other important attributes </t>
+  </si>
+  <si>
+    <t>Test for each individual function in a separate py file</t>
+  </si>
+  <si>
+    <t>While testing make a structures notebook</t>
+  </si>
+  <si>
+    <t>The structure could be installing dependencies, importing dependencies, config file (either import or evrything defined in a cell), importing tables and cleaning them, then lastly testing out the individual functions of the module one by one</t>
+  </si>
+  <si>
+    <t>Make functions of a module both in pandas and pyspark</t>
   </si>
 </sst>
 </file>
@@ -404,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,65 +446,91 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="A9:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding some more points to best practises excel
</commit_message>
<xml_diff>
--- a/Best Practises/General guidelines for every project.xlsx
+++ b/Best Practises/General guidelines for every project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankush.bhardwaj\Desktop\Personal\Miscellaneous\Best Practises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A889B6-C183-4EBB-A594-6EE80FEB8E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BC74FA-A276-4D15-8B83-44B30CA395E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">Main Point </t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Line level comment</t>
-  </si>
-  <si>
-    <t>Some folders are src, data, notebooks etc</t>
   </si>
   <si>
     <t>Make an excel detailing everyday work with date</t>
@@ -73,16 +70,47 @@
 input data size and other important attributes </t>
   </si>
   <si>
-    <t>Test for each individual function in a separate py file</t>
-  </si>
-  <si>
     <t>While testing make a structures notebook</t>
   </si>
   <si>
     <t>The structure could be installing dependencies, importing dependencies, config file (either import or evrything defined in a cell), importing tables and cleaning them, then lastly testing out the individual functions of the module one by one</t>
   </si>
   <si>
-    <t>Make functions of a module both in pandas and pyspark</t>
+    <t>Make two noteboks, one for complete testing and 
+one for testing a specific function of the py file</t>
+  </si>
+  <si>
+    <t>The specific function testing notebook is for other people benefit because the would find the complete workflow notebook to be lengthy and unclean</t>
+  </si>
+  <si>
+    <t>In the specific function testing notebook, do not import from py file rather paste the complete function from the py file into a cell of the notebook. People generally prefer function (that is to be tested) in the same notebook</t>
+  </si>
+  <si>
+    <t>Test for each individual functions which are in a separate py file</t>
+  </si>
+  <si>
+    <t>Make functions that are in separate py file of a module both in pandas and pyspark</t>
+  </si>
+  <si>
+    <t>To-Do</t>
+  </si>
+  <si>
+    <t>Get the TAMLAP Folder structure</t>
+  </si>
+  <si>
+    <t>Make an excel detailing all the tables used in the product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The first sheet of the excel would mention all the tables that were used or created. A breif description of the tables is also to be added
+And the subsequent sheet would be table specific where the on a single sheet a single table's columns would be mentioned, a brief about the column, some example of the data present in column etc </t>
+  </si>
+  <si>
+    <t>Some folders are src, config ,data, notebooks, 
+deploy, requiremnts.txt etc</t>
+  </si>
+  <si>
+    <t>Dependencies to be installed from requirements.txt and 
+versions of the dependencies also to be mentioned in the requiremnets file</t>
   </si>
 </sst>
 </file>
@@ -126,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -139,6 +167,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -420,117 +451,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:B15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="74.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="85.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="B11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
+      <c r="B14" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A9:A14"/>
+  <mergeCells count="2">
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A12:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>